<commit_message>
Import số liệu từ kho bạc nhà nước sửa danh sách khai thuế + import ds khai thuế
</commit_message>
<xml_diff>
--- a/TelerikWebApp1/Template/DanhSachKhaiThue_Import.xlsx
+++ b/TelerikWebApp1/Template/DanhSachKhaiThue_Import.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Mã số thuế</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>Ngày khai thuế</t>
-  </si>
-  <si>
-    <t>Lần khai thuế</t>
   </si>
   <si>
     <t>Kinh doanh từ giờ</t>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>ngaykhaithue</t>
-  </si>
-  <si>
-    <t>lan</t>
   </si>
   <si>
     <t>TuGio</t>
@@ -555,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L250"/>
+  <dimension ref="A1:K250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,13 +560,12 @@
     <col min="1" max="1" width="18.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -582,10 +575,10 @@
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -606,49 +599,43 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
@@ -657,12 +644,11 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10"/>
@@ -671,12 +657,11 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10"/>
@@ -685,12 +670,11 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10"/>
@@ -699,12 +683,11 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="1"/>
       <c r="C7" s="10"/>
@@ -713,12 +696,11 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10"/>
@@ -727,12 +709,11 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
@@ -741,12 +722,11 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
@@ -755,12 +735,11 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
@@ -769,12 +748,11 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="1"/>
       <c r="C12" s="10"/>
@@ -783,12 +761,11 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="1"/>
       <c r="C13" s="10"/>
@@ -797,12 +774,11 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="1"/>
       <c r="C14" s="10"/>
@@ -811,12 +787,11 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="1"/>
       <c r="C15" s="10"/>
@@ -825,12 +800,11 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="1"/>
       <c r="C16" s="10"/>
@@ -839,12 +813,11 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10"/>
@@ -853,12 +826,11 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="1"/>
       <c r="C18" s="10"/>
@@ -867,12 +839,11 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="1"/>
       <c r="C19" s="10"/>
@@ -881,12 +852,11 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="1"/>
       <c r="C20" s="10"/>
@@ -895,12 +865,11 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="1"/>
       <c r="C21" s="10"/>
@@ -909,12 +878,11 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="1"/>
       <c r="C22" s="10"/>
@@ -923,12 +891,11 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="1"/>
       <c r="C23" s="10"/>
@@ -937,12 +904,11 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="1"/>
       <c r="C24" s="10"/>
@@ -954,9 +920,8 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="1"/>
       <c r="C25" s="10"/>
@@ -968,9 +933,8 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="1"/>
       <c r="C26" s="10"/>
@@ -982,9 +946,8 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="1"/>
       <c r="C27" s="10"/>
@@ -996,9 +959,8 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="1"/>
       <c r="C28" s="10"/>
@@ -1010,9 +972,8 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="1"/>
       <c r="C29" s="10"/>
@@ -1024,9 +985,8 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="1"/>
       <c r="C30" s="10"/>
@@ -1038,9 +998,8 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="1"/>
       <c r="C31" s="10"/>
@@ -1052,9 +1011,8 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="1"/>
       <c r="C32" s="10"/>
@@ -1066,9 +1024,8 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="1"/>
       <c r="C33" s="10"/>
@@ -1080,9 +1037,8 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="1"/>
       <c r="C34" s="10"/>
@@ -1094,9 +1050,8 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="1"/>
       <c r="C35" s="10"/>
@@ -1108,9 +1063,8 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="1"/>
       <c r="C36" s="10"/>
@@ -1122,9 +1076,8 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="1"/>
       <c r="C37" s="10"/>
@@ -1136,9 +1089,8 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="1"/>
       <c r="C38" s="10"/>
@@ -1150,9 +1102,8 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="1"/>
       <c r="C39" s="10"/>
@@ -1164,9 +1115,8 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="1"/>
       <c r="C40" s="10"/>
@@ -1178,9 +1128,8 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="1"/>
       <c r="C41" s="10"/>
@@ -1192,9 +1141,8 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="1"/>
       <c r="C42" s="10"/>
@@ -1206,9 +1154,8 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="1"/>
       <c r="C43" s="10"/>
@@ -1220,9 +1167,8 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="1"/>
       <c r="C44" s="10"/>
@@ -1234,9 +1180,8 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="1"/>
       <c r="C45" s="10"/>
@@ -1248,9 +1193,8 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
@@ -1262,9 +1206,8 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
@@ -1276,9 +1219,8 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
@@ -1290,9 +1232,8 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
@@ -1304,9 +1245,8 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
@@ -1318,9 +1258,8 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
@@ -1332,9 +1271,8 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
@@ -1346,9 +1284,8 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
@@ -1360,9 +1297,8 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
@@ -1374,9 +1310,8 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
@@ -1388,9 +1323,8 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
@@ -1402,9 +1336,8 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="1"/>
       <c r="C57" s="10"/>
@@ -1416,9 +1349,8 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
@@ -1430,9 +1362,8 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
@@ -1444,9 +1375,8 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="1"/>
       <c r="C60" s="10"/>
@@ -1458,9 +1388,8 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
@@ -1472,9 +1401,8 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="1"/>
       <c r="C62" s="10"/>
@@ -1486,9 +1414,8 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="1"/>
       <c r="C63" s="10"/>
@@ -1500,9 +1427,8 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="1"/>
       <c r="C64" s="10"/>
@@ -1514,9 +1440,8 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="1"/>
       <c r="C65" s="10"/>
@@ -1528,9 +1453,8 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="1"/>
       <c r="C66" s="10"/>
@@ -1542,9 +1466,8 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="1"/>
       <c r="C67" s="10"/>
@@ -1556,9 +1479,8 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="1"/>
       <c r="C68" s="10"/>
@@ -1570,9 +1492,8 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="1"/>
       <c r="C69" s="10"/>
@@ -1584,9 +1505,8 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="1"/>
       <c r="C70" s="10"/>
@@ -1598,9 +1518,8 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="1"/>
       <c r="C71" s="10"/>
@@ -1612,9 +1531,8 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="1"/>
       <c r="C72" s="10"/>
@@ -1626,9 +1544,8 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="1"/>
       <c r="C73" s="10"/>
@@ -1640,9 +1557,8 @@
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="1"/>
       <c r="C74" s="10"/>
@@ -1654,9 +1570,8 @@
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="1"/>
       <c r="C75" s="10"/>
@@ -1668,9 +1583,8 @@
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="1"/>
       <c r="C76" s="10"/>
@@ -1682,9 +1596,8 @@
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="1"/>
       <c r="C77" s="10"/>
@@ -1696,9 +1609,8 @@
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
       <c r="B78" s="1"/>
       <c r="C78" s="10"/>
@@ -1710,9 +1622,8 @@
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="1"/>
       <c r="C79" s="10"/>
@@ -1724,9 +1635,8 @@
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="1"/>
       <c r="C80" s="10"/>
@@ -1738,9 +1648,8 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="1"/>
       <c r="C81" s="10"/>
@@ -1752,9 +1661,8 @@
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="1"/>
       <c r="C82" s="10"/>
@@ -1766,9 +1674,8 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
-      <c r="L82" s="1"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="1"/>
       <c r="C83" s="10"/>
@@ -1780,9 +1687,8 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
       <c r="B84" s="1"/>
       <c r="C84" s="10"/>
@@ -1794,9 +1700,8 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
-      <c r="L84" s="1"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="1"/>
       <c r="C85" s="10"/>
@@ -1808,9 +1713,8 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
-      <c r="L85" s="1"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="10"/>
       <c r="B86" s="1"/>
       <c r="C86" s="10"/>
@@ -1822,9 +1726,8 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
-      <c r="L86" s="1"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="1"/>
       <c r="C87" s="10"/>
@@ -1836,9 +1739,8 @@
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="1"/>
       <c r="C88" s="10"/>
@@ -1850,9 +1752,8 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
-      <c r="L88" s="1"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="1"/>
       <c r="C89" s="10"/>
@@ -1864,9 +1765,8 @@
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="1"/>
       <c r="C90" s="10"/>
@@ -1878,9 +1778,8 @@
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="10"/>
       <c r="B91" s="1"/>
       <c r="C91" s="10"/>
@@ -1892,9 +1791,8 @@
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
-      <c r="L91" s="1"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
       <c r="B92" s="1"/>
       <c r="C92" s="10"/>
@@ -1906,9 +1804,8 @@
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="1"/>
       <c r="C93" s="10"/>
@@ -1920,9 +1817,8 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
-      <c r="L93" s="1"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="10"/>
       <c r="B94" s="1"/>
       <c r="C94" s="10"/>
@@ -1934,9 +1830,8 @@
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
-      <c r="L94" s="1"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="B95" s="1"/>
       <c r="C95" s="10"/>
@@ -1948,9 +1843,8 @@
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
-      <c r="L95" s="1"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="1"/>
       <c r="C96" s="10"/>
@@ -1962,9 +1856,8 @@
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
-      <c r="L96" s="1"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="1"/>
       <c r="C97" s="10"/>
@@ -1976,9 +1869,8 @@
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
-      <c r="L97" s="1"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="1"/>
       <c r="C98" s="10"/>
@@ -1990,9 +1882,8 @@
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
-      <c r="L98" s="1"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
       <c r="B99" s="1"/>
       <c r="C99" s="10"/>
@@ -2004,9 +1895,8 @@
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="1"/>
       <c r="C100" s="10"/>
@@ -2018,9 +1908,8 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
       <c r="B101" s="1"/>
       <c r="C101" s="10"/>
@@ -2032,9 +1921,8 @@
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="10"/>
       <c r="B102" s="1"/>
       <c r="C102" s="10"/>
@@ -2046,9 +1934,8 @@
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
       <c r="B103" s="1"/>
       <c r="C103" s="10"/>
@@ -2060,9 +1947,8 @@
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
       <c r="B104" s="1"/>
       <c r="C104" s="10"/>
@@ -2074,9 +1960,8 @@
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
       <c r="B105" s="1"/>
       <c r="C105" s="10"/>
@@ -2088,9 +1973,8 @@
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
-      <c r="L105" s="1"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="1"/>
       <c r="C106" s="10"/>
@@ -2102,9 +1986,8 @@
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
-      <c r="L106" s="1"/>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="10"/>
       <c r="B107" s="1"/>
       <c r="C107" s="10"/>
@@ -2116,9 +1999,8 @@
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
-      <c r="L107" s="1"/>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="10"/>
       <c r="B108" s="1"/>
       <c r="C108" s="10"/>
@@ -2130,9 +2012,8 @@
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
-      <c r="L108" s="1"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
       <c r="B109" s="1"/>
       <c r="C109" s="10"/>
@@ -2144,9 +2025,8 @@
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
-      <c r="L109" s="1"/>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="10"/>
       <c r="B110" s="1"/>
       <c r="C110" s="10"/>
@@ -2158,9 +2038,8 @@
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
-      <c r="L110" s="1"/>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
       <c r="B111" s="1"/>
       <c r="C111" s="10"/>
@@ -2172,9 +2051,8 @@
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
-      <c r="L111" s="1"/>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="1"/>
       <c r="C112" s="10"/>
@@ -2186,9 +2064,8 @@
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
-      <c r="L112" s="1"/>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
       <c r="B113" s="1"/>
       <c r="C113" s="10"/>
@@ -2200,9 +2077,8 @@
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
-      <c r="L113" s="1"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="1"/>
       <c r="C114" s="10"/>
@@ -2214,9 +2090,8 @@
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
-      <c r="L114" s="1"/>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="10"/>
       <c r="B115" s="1"/>
       <c r="C115" s="10"/>
@@ -2228,9 +2103,8 @@
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
-      <c r="L115" s="1"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="10"/>
       <c r="B116" s="1"/>
       <c r="C116" s="10"/>
@@ -2242,9 +2116,8 @@
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
-      <c r="L116" s="1"/>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="10"/>
       <c r="B117" s="1"/>
       <c r="C117" s="10"/>
@@ -2256,9 +2129,8 @@
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
-      <c r="L117" s="1"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="10"/>
       <c r="B118" s="1"/>
       <c r="C118" s="10"/>
@@ -2270,9 +2142,8 @@
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
-      <c r="L118" s="1"/>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="10"/>
       <c r="B119" s="1"/>
       <c r="C119" s="10"/>
@@ -2284,9 +2155,8 @@
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
-      <c r="L119" s="1"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="1"/>
       <c r="C120" s="10"/>
@@ -2298,9 +2168,8 @@
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
-      <c r="L120" s="1"/>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
       <c r="B121" s="1"/>
       <c r="C121" s="10"/>
@@ -2312,9 +2181,8 @@
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
-      <c r="L121" s="1"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="1"/>
       <c r="C122" s="10"/>
@@ -2326,9 +2194,8 @@
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
-      <c r="L122" s="1"/>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="10"/>
       <c r="B123" s="1"/>
       <c r="C123" s="10"/>
@@ -2340,9 +2207,8 @@
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
-      <c r="L123" s="1"/>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="10"/>
       <c r="B124" s="1"/>
       <c r="C124" s="10"/>
@@ -2354,9 +2220,8 @@
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
-      <c r="L124" s="1"/>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="10"/>
       <c r="B125" s="1"/>
       <c r="C125" s="10"/>
@@ -2368,9 +2233,8 @@
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
-      <c r="L125" s="1"/>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
       <c r="B126" s="1"/>
       <c r="C126" s="10"/>
@@ -2382,9 +2246,8 @@
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
-      <c r="L126" s="1"/>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="10"/>
       <c r="B127" s="1"/>
       <c r="C127" s="10"/>
@@ -2396,9 +2259,8 @@
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
-      <c r="L127" s="1"/>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="10"/>
       <c r="B128" s="1"/>
       <c r="C128" s="10"/>
@@ -2410,9 +2272,8 @@
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
-      <c r="L128" s="1"/>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="10"/>
       <c r="B129" s="1"/>
       <c r="C129" s="10"/>
@@ -2424,9 +2285,8 @@
       <c r="I129" s="1"/>
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
-      <c r="L129" s="1"/>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
       <c r="B130" s="1"/>
       <c r="C130" s="10"/>
@@ -2438,9 +2298,8 @@
       <c r="I130" s="1"/>
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
-      <c r="L130" s="1"/>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="10"/>
       <c r="B131" s="1"/>
       <c r="C131" s="10"/>
@@ -2452,9 +2311,8 @@
       <c r="I131" s="1"/>
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
-      <c r="L131" s="1"/>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="10"/>
       <c r="B132" s="1"/>
       <c r="C132" s="10"/>
@@ -2466,9 +2324,8 @@
       <c r="I132" s="1"/>
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
-      <c r="L132" s="1"/>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="10"/>
       <c r="B133" s="1"/>
       <c r="C133" s="10"/>
@@ -2480,9 +2337,8 @@
       <c r="I133" s="1"/>
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
-      <c r="L133" s="1"/>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="10"/>
       <c r="B134" s="1"/>
       <c r="C134" s="10"/>
@@ -2494,9 +2350,8 @@
       <c r="I134" s="1"/>
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
-      <c r="L134" s="1"/>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="10"/>
       <c r="B135" s="1"/>
       <c r="C135" s="10"/>
@@ -2508,9 +2363,8 @@
       <c r="I135" s="1"/>
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
-      <c r="L135" s="1"/>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="10"/>
       <c r="B136" s="1"/>
       <c r="C136" s="10"/>
@@ -2522,9 +2376,8 @@
       <c r="I136" s="1"/>
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
-      <c r="L136" s="1"/>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="10"/>
       <c r="B137" s="1"/>
       <c r="C137" s="10"/>
@@ -2536,9 +2389,8 @@
       <c r="I137" s="1"/>
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
-      <c r="L137" s="1"/>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="10"/>
       <c r="B138" s="1"/>
       <c r="C138" s="10"/>
@@ -2550,9 +2402,8 @@
       <c r="I138" s="1"/>
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
-      <c r="L138" s="1"/>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="10"/>
       <c r="B139" s="1"/>
       <c r="C139" s="10"/>
@@ -2564,9 +2415,8 @@
       <c r="I139" s="1"/>
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
-      <c r="L139" s="1"/>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="10"/>
       <c r="B140" s="1"/>
       <c r="C140" s="10"/>
@@ -2578,9 +2428,8 @@
       <c r="I140" s="1"/>
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
-      <c r="L140" s="1"/>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="10"/>
       <c r="B141" s="1"/>
       <c r="C141" s="10"/>
@@ -2592,9 +2441,8 @@
       <c r="I141" s="1"/>
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
-      <c r="L141" s="1"/>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="10"/>
       <c r="B142" s="1"/>
       <c r="C142" s="10"/>
@@ -2606,9 +2454,8 @@
       <c r="I142" s="1"/>
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
-      <c r="L142" s="1"/>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="10"/>
       <c r="B143" s="1"/>
       <c r="C143" s="10"/>
@@ -2620,9 +2467,8 @@
       <c r="I143" s="1"/>
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
-      <c r="L143" s="1"/>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="10"/>
       <c r="B144" s="1"/>
       <c r="C144" s="10"/>
@@ -2634,9 +2480,8 @@
       <c r="I144" s="1"/>
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
-      <c r="L144" s="1"/>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="10"/>
       <c r="B145" s="1"/>
       <c r="C145" s="10"/>
@@ -2648,9 +2493,8 @@
       <c r="I145" s="1"/>
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
-      <c r="L145" s="1"/>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="10"/>
       <c r="B146" s="1"/>
       <c r="C146" s="10"/>
@@ -2662,9 +2506,8 @@
       <c r="I146" s="1"/>
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
-      <c r="L146" s="1"/>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="10"/>
       <c r="B147" s="1"/>
       <c r="C147" s="10"/>
@@ -2676,9 +2519,8 @@
       <c r="I147" s="1"/>
       <c r="J147" s="1"/>
       <c r="K147" s="1"/>
-      <c r="L147" s="1"/>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="10"/>
       <c r="B148" s="1"/>
       <c r="C148" s="10"/>
@@ -2690,9 +2532,8 @@
       <c r="I148" s="1"/>
       <c r="J148" s="1"/>
       <c r="K148" s="1"/>
-      <c r="L148" s="1"/>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="10"/>
       <c r="B149" s="1"/>
       <c r="C149" s="10"/>
@@ -2704,9 +2545,8 @@
       <c r="I149" s="1"/>
       <c r="J149" s="1"/>
       <c r="K149" s="1"/>
-      <c r="L149" s="1"/>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="10"/>
       <c r="B150" s="1"/>
       <c r="C150" s="10"/>
@@ -2718,9 +2558,8 @@
       <c r="I150" s="1"/>
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
-      <c r="L150" s="1"/>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="10"/>
       <c r="B151" s="1"/>
       <c r="C151" s="10"/>
@@ -2732,9 +2571,8 @@
       <c r="I151" s="1"/>
       <c r="J151" s="1"/>
       <c r="K151" s="1"/>
-      <c r="L151" s="1"/>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="10"/>
       <c r="B152" s="1"/>
       <c r="C152" s="10"/>
@@ -2746,9 +2584,8 @@
       <c r="I152" s="1"/>
       <c r="J152" s="1"/>
       <c r="K152" s="1"/>
-      <c r="L152" s="1"/>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="10"/>
       <c r="B153" s="1"/>
       <c r="C153" s="10"/>
@@ -2760,9 +2597,8 @@
       <c r="I153" s="1"/>
       <c r="J153" s="1"/>
       <c r="K153" s="1"/>
-      <c r="L153" s="1"/>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="10"/>
       <c r="B154" s="1"/>
       <c r="C154" s="10"/>
@@ -2774,9 +2610,8 @@
       <c r="I154" s="1"/>
       <c r="J154" s="1"/>
       <c r="K154" s="1"/>
-      <c r="L154" s="1"/>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="10"/>
       <c r="B155" s="1"/>
       <c r="C155" s="10"/>
@@ -2788,9 +2623,8 @@
       <c r="I155" s="1"/>
       <c r="J155" s="1"/>
       <c r="K155" s="1"/>
-      <c r="L155" s="1"/>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="10"/>
       <c r="B156" s="1"/>
       <c r="C156" s="10"/>
@@ -2802,9 +2636,8 @@
       <c r="I156" s="1"/>
       <c r="J156" s="1"/>
       <c r="K156" s="1"/>
-      <c r="L156" s="1"/>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="10"/>
       <c r="B157" s="1"/>
       <c r="C157" s="10"/>
@@ -2816,9 +2649,8 @@
       <c r="I157" s="1"/>
       <c r="J157" s="1"/>
       <c r="K157" s="1"/>
-      <c r="L157" s="1"/>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="10"/>
       <c r="B158" s="1"/>
       <c r="C158" s="10"/>
@@ -2830,9 +2662,8 @@
       <c r="I158" s="1"/>
       <c r="J158" s="1"/>
       <c r="K158" s="1"/>
-      <c r="L158" s="1"/>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="10"/>
       <c r="B159" s="1"/>
       <c r="C159" s="10"/>
@@ -2844,9 +2675,8 @@
       <c r="I159" s="1"/>
       <c r="J159" s="1"/>
       <c r="K159" s="1"/>
-      <c r="L159" s="1"/>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="10"/>
       <c r="B160" s="1"/>
       <c r="C160" s="10"/>
@@ -2858,9 +2688,8 @@
       <c r="I160" s="1"/>
       <c r="J160" s="1"/>
       <c r="K160" s="1"/>
-      <c r="L160" s="1"/>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="10"/>
       <c r="B161" s="1"/>
       <c r="C161" s="10"/>
@@ -2872,9 +2701,8 @@
       <c r="I161" s="1"/>
       <c r="J161" s="1"/>
       <c r="K161" s="1"/>
-      <c r="L161" s="1"/>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="10"/>
       <c r="B162" s="1"/>
       <c r="C162" s="10"/>
@@ -2886,9 +2714,8 @@
       <c r="I162" s="1"/>
       <c r="J162" s="1"/>
       <c r="K162" s="1"/>
-      <c r="L162" s="1"/>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="10"/>
       <c r="B163" s="1"/>
       <c r="C163" s="10"/>
@@ -2900,9 +2727,8 @@
       <c r="I163" s="1"/>
       <c r="J163" s="1"/>
       <c r="K163" s="1"/>
-      <c r="L163" s="1"/>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="10"/>
       <c r="B164" s="1"/>
       <c r="C164" s="10"/>
@@ -2914,9 +2740,8 @@
       <c r="I164" s="1"/>
       <c r="J164" s="1"/>
       <c r="K164" s="1"/>
-      <c r="L164" s="1"/>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="10"/>
       <c r="B165" s="1"/>
       <c r="C165" s="10"/>
@@ -2928,9 +2753,8 @@
       <c r="I165" s="1"/>
       <c r="J165" s="1"/>
       <c r="K165" s="1"/>
-      <c r="L165" s="1"/>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="10"/>
       <c r="B166" s="1"/>
       <c r="C166" s="10"/>
@@ -2942,9 +2766,8 @@
       <c r="I166" s="1"/>
       <c r="J166" s="1"/>
       <c r="K166" s="1"/>
-      <c r="L166" s="1"/>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="10"/>
       <c r="B167" s="1"/>
       <c r="C167" s="10"/>
@@ -2956,9 +2779,8 @@
       <c r="I167" s="1"/>
       <c r="J167" s="1"/>
       <c r="K167" s="1"/>
-      <c r="L167" s="1"/>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="10"/>
       <c r="B168" s="1"/>
       <c r="C168" s="10"/>
@@ -2970,9 +2792,8 @@
       <c r="I168" s="1"/>
       <c r="J168" s="1"/>
       <c r="K168" s="1"/>
-      <c r="L168" s="1"/>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="10"/>
       <c r="B169" s="1"/>
       <c r="C169" s="10"/>
@@ -2984,9 +2805,8 @@
       <c r="I169" s="1"/>
       <c r="J169" s="1"/>
       <c r="K169" s="1"/>
-      <c r="L169" s="1"/>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="10"/>
       <c r="B170" s="1"/>
       <c r="C170" s="10"/>
@@ -2998,9 +2818,8 @@
       <c r="I170" s="1"/>
       <c r="J170" s="1"/>
       <c r="K170" s="1"/>
-      <c r="L170" s="1"/>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="10"/>
       <c r="B171" s="1"/>
       <c r="C171" s="10"/>
@@ -3012,9 +2831,8 @@
       <c r="I171" s="1"/>
       <c r="J171" s="1"/>
       <c r="K171" s="1"/>
-      <c r="L171" s="1"/>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="10"/>
       <c r="B172" s="1"/>
       <c r="C172" s="10"/>
@@ -3026,9 +2844,8 @@
       <c r="I172" s="1"/>
       <c r="J172" s="1"/>
       <c r="K172" s="1"/>
-      <c r="L172" s="1"/>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="10"/>
       <c r="B173" s="1"/>
       <c r="C173" s="10"/>
@@ -3040,9 +2857,8 @@
       <c r="I173" s="1"/>
       <c r="J173" s="1"/>
       <c r="K173" s="1"/>
-      <c r="L173" s="1"/>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="10"/>
       <c r="B174" s="1"/>
       <c r="C174" s="10"/>
@@ -3054,9 +2870,8 @@
       <c r="I174" s="1"/>
       <c r="J174" s="1"/>
       <c r="K174" s="1"/>
-      <c r="L174" s="1"/>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="10"/>
       <c r="B175" s="1"/>
       <c r="C175" s="10"/>
@@ -3068,9 +2883,8 @@
       <c r="I175" s="1"/>
       <c r="J175" s="1"/>
       <c r="K175" s="1"/>
-      <c r="L175" s="1"/>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="10"/>
       <c r="B176" s="1"/>
       <c r="C176" s="10"/>
@@ -3082,9 +2896,8 @@
       <c r="I176" s="1"/>
       <c r="J176" s="1"/>
       <c r="K176" s="1"/>
-      <c r="L176" s="1"/>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="10"/>
       <c r="B177" s="1"/>
       <c r="C177" s="10"/>
@@ -3096,9 +2909,8 @@
       <c r="I177" s="1"/>
       <c r="J177" s="1"/>
       <c r="K177" s="1"/>
-      <c r="L177" s="1"/>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="10"/>
       <c r="B178" s="1"/>
       <c r="C178" s="10"/>
@@ -3110,9 +2922,8 @@
       <c r="I178" s="1"/>
       <c r="J178" s="1"/>
       <c r="K178" s="1"/>
-      <c r="L178" s="1"/>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="10"/>
       <c r="B179" s="1"/>
       <c r="C179" s="10"/>
@@ -3124,9 +2935,8 @@
       <c r="I179" s="1"/>
       <c r="J179" s="1"/>
       <c r="K179" s="1"/>
-      <c r="L179" s="1"/>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="10"/>
       <c r="B180" s="1"/>
       <c r="C180" s="10"/>
@@ -3138,9 +2948,8 @@
       <c r="I180" s="1"/>
       <c r="J180" s="1"/>
       <c r="K180" s="1"/>
-      <c r="L180" s="1"/>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="10"/>
       <c r="B181" s="1"/>
       <c r="C181" s="10"/>
@@ -3152,9 +2961,8 @@
       <c r="I181" s="1"/>
       <c r="J181" s="1"/>
       <c r="K181" s="1"/>
-      <c r="L181" s="1"/>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="10"/>
       <c r="B182" s="1"/>
       <c r="C182" s="10"/>
@@ -3166,9 +2974,8 @@
       <c r="I182" s="1"/>
       <c r="J182" s="1"/>
       <c r="K182" s="1"/>
-      <c r="L182" s="1"/>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="10"/>
       <c r="B183" s="1"/>
       <c r="C183" s="10"/>
@@ -3180,9 +2987,8 @@
       <c r="I183" s="1"/>
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
-      <c r="L183" s="1"/>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="10"/>
       <c r="B184" s="1"/>
       <c r="C184" s="10"/>
@@ -3194,9 +3000,8 @@
       <c r="I184" s="1"/>
       <c r="J184" s="1"/>
       <c r="K184" s="1"/>
-      <c r="L184" s="1"/>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="10"/>
       <c r="B185" s="1"/>
       <c r="C185" s="10"/>
@@ -3208,9 +3013,8 @@
       <c r="I185" s="1"/>
       <c r="J185" s="1"/>
       <c r="K185" s="1"/>
-      <c r="L185" s="1"/>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="10"/>
       <c r="B186" s="1"/>
       <c r="C186" s="10"/>
@@ -3222,9 +3026,8 @@
       <c r="I186" s="1"/>
       <c r="J186" s="1"/>
       <c r="K186" s="1"/>
-      <c r="L186" s="1"/>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="10"/>
       <c r="B187" s="1"/>
       <c r="C187" s="10"/>
@@ -3236,9 +3039,8 @@
       <c r="I187" s="1"/>
       <c r="J187" s="1"/>
       <c r="K187" s="1"/>
-      <c r="L187" s="1"/>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="10"/>
       <c r="B188" s="1"/>
       <c r="C188" s="10"/>
@@ -3250,9 +3052,8 @@
       <c r="I188" s="1"/>
       <c r="J188" s="1"/>
       <c r="K188" s="1"/>
-      <c r="L188" s="1"/>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="10"/>
       <c r="B189" s="1"/>
       <c r="C189" s="10"/>
@@ -3264,9 +3065,8 @@
       <c r="I189" s="1"/>
       <c r="J189" s="1"/>
       <c r="K189" s="1"/>
-      <c r="L189" s="1"/>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="10"/>
       <c r="B190" s="1"/>
       <c r="C190" s="10"/>
@@ -3278,9 +3078,8 @@
       <c r="I190" s="1"/>
       <c r="J190" s="1"/>
       <c r="K190" s="1"/>
-      <c r="L190" s="1"/>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="10"/>
       <c r="B191" s="1"/>
       <c r="C191" s="10"/>
@@ -3292,9 +3091,8 @@
       <c r="I191" s="1"/>
       <c r="J191" s="1"/>
       <c r="K191" s="1"/>
-      <c r="L191" s="1"/>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="10"/>
       <c r="B192" s="1"/>
       <c r="C192" s="10"/>
@@ -3306,9 +3104,8 @@
       <c r="I192" s="1"/>
       <c r="J192" s="1"/>
       <c r="K192" s="1"/>
-      <c r="L192" s="1"/>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="10"/>
       <c r="B193" s="1"/>
       <c r="C193" s="10"/>
@@ -3320,9 +3117,8 @@
       <c r="I193" s="1"/>
       <c r="J193" s="1"/>
       <c r="K193" s="1"/>
-      <c r="L193" s="1"/>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="10"/>
       <c r="B194" s="1"/>
       <c r="C194" s="10"/>
@@ -3334,9 +3130,8 @@
       <c r="I194" s="1"/>
       <c r="J194" s="1"/>
       <c r="K194" s="1"/>
-      <c r="L194" s="1"/>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="10"/>
       <c r="B195" s="1"/>
       <c r="C195" s="10"/>
@@ -3348,9 +3143,8 @@
       <c r="I195" s="1"/>
       <c r="J195" s="1"/>
       <c r="K195" s="1"/>
-      <c r="L195" s="1"/>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="10"/>
       <c r="B196" s="1"/>
       <c r="C196" s="10"/>
@@ -3362,9 +3156,8 @@
       <c r="I196" s="1"/>
       <c r="J196" s="1"/>
       <c r="K196" s="1"/>
-      <c r="L196" s="1"/>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="10"/>
       <c r="B197" s="1"/>
       <c r="C197" s="10"/>
@@ -3376,9 +3169,8 @@
       <c r="I197" s="1"/>
       <c r="J197" s="1"/>
       <c r="K197" s="1"/>
-      <c r="L197" s="1"/>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="10"/>
       <c r="B198" s="1"/>
       <c r="C198" s="10"/>
@@ -3390,9 +3182,8 @@
       <c r="I198" s="1"/>
       <c r="J198" s="1"/>
       <c r="K198" s="1"/>
-      <c r="L198" s="1"/>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="10"/>
       <c r="B199" s="1"/>
       <c r="C199" s="10"/>
@@ -3404,9 +3195,8 @@
       <c r="I199" s="1"/>
       <c r="J199" s="1"/>
       <c r="K199" s="1"/>
-      <c r="L199" s="1"/>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="10"/>
       <c r="B200" s="1"/>
       <c r="C200" s="10"/>
@@ -3418,9 +3208,8 @@
       <c r="I200" s="1"/>
       <c r="J200" s="1"/>
       <c r="K200" s="1"/>
-      <c r="L200" s="1"/>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="10"/>
       <c r="B201" s="1"/>
       <c r="C201" s="10"/>
@@ -3432,9 +3221,8 @@
       <c r="I201" s="1"/>
       <c r="J201" s="1"/>
       <c r="K201" s="1"/>
-      <c r="L201" s="1"/>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="10"/>
       <c r="B202" s="1"/>
       <c r="C202" s="10"/>
@@ -3446,9 +3234,8 @@
       <c r="I202" s="1"/>
       <c r="J202" s="1"/>
       <c r="K202" s="1"/>
-      <c r="L202" s="1"/>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="10"/>
       <c r="B203" s="1"/>
       <c r="C203" s="10"/>
@@ -3460,9 +3247,8 @@
       <c r="I203" s="1"/>
       <c r="J203" s="1"/>
       <c r="K203" s="1"/>
-      <c r="L203" s="1"/>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="10"/>
       <c r="B204" s="1"/>
       <c r="C204" s="10"/>
@@ -3474,9 +3260,8 @@
       <c r="I204" s="1"/>
       <c r="J204" s="1"/>
       <c r="K204" s="1"/>
-      <c r="L204" s="1"/>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="10"/>
       <c r="B205" s="1"/>
       <c r="C205" s="10"/>
@@ -3488,9 +3273,8 @@
       <c r="I205" s="1"/>
       <c r="J205" s="1"/>
       <c r="K205" s="1"/>
-      <c r="L205" s="1"/>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="10"/>
       <c r="B206" s="1"/>
       <c r="C206" s="10"/>
@@ -3502,9 +3286,8 @@
       <c r="I206" s="1"/>
       <c r="J206" s="1"/>
       <c r="K206" s="1"/>
-      <c r="L206" s="1"/>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="10"/>
       <c r="B207" s="1"/>
       <c r="C207" s="10"/>
@@ -3516,9 +3299,8 @@
       <c r="I207" s="1"/>
       <c r="J207" s="1"/>
       <c r="K207" s="1"/>
-      <c r="L207" s="1"/>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="10"/>
       <c r="B208" s="1"/>
       <c r="C208" s="10"/>
@@ -3530,9 +3312,8 @@
       <c r="I208" s="1"/>
       <c r="J208" s="1"/>
       <c r="K208" s="1"/>
-      <c r="L208" s="1"/>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="10"/>
       <c r="B209" s="1"/>
       <c r="C209" s="10"/>
@@ -3544,9 +3325,8 @@
       <c r="I209" s="1"/>
       <c r="J209" s="1"/>
       <c r="K209" s="1"/>
-      <c r="L209" s="1"/>
-    </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="10"/>
       <c r="B210" s="1"/>
       <c r="C210" s="10"/>
@@ -3558,9 +3338,8 @@
       <c r="I210" s="1"/>
       <c r="J210" s="1"/>
       <c r="K210" s="1"/>
-      <c r="L210" s="1"/>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="10"/>
       <c r="B211" s="1"/>
       <c r="C211" s="10"/>
@@ -3572,9 +3351,8 @@
       <c r="I211" s="1"/>
       <c r="J211" s="1"/>
       <c r="K211" s="1"/>
-      <c r="L211" s="1"/>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="10"/>
       <c r="B212" s="1"/>
       <c r="C212" s="10"/>
@@ -3586,9 +3364,8 @@
       <c r="I212" s="1"/>
       <c r="J212" s="1"/>
       <c r="K212" s="1"/>
-      <c r="L212" s="1"/>
-    </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="10"/>
       <c r="B213" s="1"/>
       <c r="C213" s="10"/>
@@ -3600,9 +3377,8 @@
       <c r="I213" s="1"/>
       <c r="J213" s="1"/>
       <c r="K213" s="1"/>
-      <c r="L213" s="1"/>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="10"/>
       <c r="B214" s="1"/>
       <c r="C214" s="10"/>
@@ -3614,9 +3390,8 @@
       <c r="I214" s="1"/>
       <c r="J214" s="1"/>
       <c r="K214" s="1"/>
-      <c r="L214" s="1"/>
-    </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="10"/>
       <c r="B215" s="1"/>
       <c r="C215" s="10"/>
@@ -3628,9 +3403,8 @@
       <c r="I215" s="1"/>
       <c r="J215" s="1"/>
       <c r="K215" s="1"/>
-      <c r="L215" s="1"/>
-    </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="10"/>
       <c r="B216" s="1"/>
       <c r="C216" s="10"/>
@@ -3642,9 +3416,8 @@
       <c r="I216" s="1"/>
       <c r="J216" s="1"/>
       <c r="K216" s="1"/>
-      <c r="L216" s="1"/>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="10"/>
       <c r="B217" s="1"/>
       <c r="C217" s="10"/>
@@ -3656,9 +3429,8 @@
       <c r="I217" s="1"/>
       <c r="J217" s="1"/>
       <c r="K217" s="1"/>
-      <c r="L217" s="1"/>
-    </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="10"/>
       <c r="B218" s="1"/>
       <c r="C218" s="10"/>
@@ -3670,9 +3442,8 @@
       <c r="I218" s="1"/>
       <c r="J218" s="1"/>
       <c r="K218" s="1"/>
-      <c r="L218" s="1"/>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="10"/>
       <c r="B219" s="1"/>
       <c r="C219" s="10"/>
@@ -3684,9 +3455,8 @@
       <c r="I219" s="1"/>
       <c r="J219" s="1"/>
       <c r="K219" s="1"/>
-      <c r="L219" s="1"/>
-    </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="10"/>
       <c r="B220" s="1"/>
       <c r="C220" s="10"/>
@@ -3698,9 +3468,8 @@
       <c r="I220" s="1"/>
       <c r="J220" s="1"/>
       <c r="K220" s="1"/>
-      <c r="L220" s="1"/>
-    </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="10"/>
       <c r="B221" s="1"/>
       <c r="C221" s="10"/>
@@ -3712,9 +3481,8 @@
       <c r="I221" s="1"/>
       <c r="J221" s="1"/>
       <c r="K221" s="1"/>
-      <c r="L221" s="1"/>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="10"/>
       <c r="B222" s="1"/>
       <c r="C222" s="10"/>
@@ -3726,9 +3494,8 @@
       <c r="I222" s="1"/>
       <c r="J222" s="1"/>
       <c r="K222" s="1"/>
-      <c r="L222" s="1"/>
-    </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="10"/>
       <c r="B223" s="1"/>
       <c r="C223" s="10"/>
@@ -3740,9 +3507,8 @@
       <c r="I223" s="1"/>
       <c r="J223" s="1"/>
       <c r="K223" s="1"/>
-      <c r="L223" s="1"/>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="10"/>
       <c r="B224" s="1"/>
       <c r="C224" s="10"/>
@@ -3754,9 +3520,8 @@
       <c r="I224" s="1"/>
       <c r="J224" s="1"/>
       <c r="K224" s="1"/>
-      <c r="L224" s="1"/>
-    </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="10"/>
       <c r="B225" s="1"/>
       <c r="C225" s="10"/>
@@ -3768,9 +3533,8 @@
       <c r="I225" s="1"/>
       <c r="J225" s="1"/>
       <c r="K225" s="1"/>
-      <c r="L225" s="1"/>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="10"/>
       <c r="B226" s="1"/>
       <c r="C226" s="10"/>
@@ -3782,9 +3546,8 @@
       <c r="I226" s="1"/>
       <c r="J226" s="1"/>
       <c r="K226" s="1"/>
-      <c r="L226" s="1"/>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="10"/>
       <c r="B227" s="1"/>
       <c r="C227" s="10"/>
@@ -3796,9 +3559,8 @@
       <c r="I227" s="1"/>
       <c r="J227" s="1"/>
       <c r="K227" s="1"/>
-      <c r="L227" s="1"/>
-    </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="10"/>
       <c r="B228" s="1"/>
       <c r="C228" s="10"/>
@@ -3810,9 +3572,8 @@
       <c r="I228" s="1"/>
       <c r="J228" s="1"/>
       <c r="K228" s="1"/>
-      <c r="L228" s="1"/>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="10"/>
       <c r="B229" s="1"/>
       <c r="C229" s="10"/>
@@ -3824,9 +3585,8 @@
       <c r="I229" s="1"/>
       <c r="J229" s="1"/>
       <c r="K229" s="1"/>
-      <c r="L229" s="1"/>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="10"/>
       <c r="B230" s="1"/>
       <c r="C230" s="10"/>
@@ -3838,9 +3598,8 @@
       <c r="I230" s="1"/>
       <c r="J230" s="1"/>
       <c r="K230" s="1"/>
-      <c r="L230" s="1"/>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="10"/>
       <c r="B231" s="1"/>
       <c r="C231" s="10"/>
@@ -3852,9 +3611,8 @@
       <c r="I231" s="1"/>
       <c r="J231" s="1"/>
       <c r="K231" s="1"/>
-      <c r="L231" s="1"/>
-    </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="10"/>
       <c r="B232" s="1"/>
       <c r="C232" s="10"/>
@@ -3866,9 +3624,8 @@
       <c r="I232" s="1"/>
       <c r="J232" s="1"/>
       <c r="K232" s="1"/>
-      <c r="L232" s="1"/>
-    </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="10"/>
       <c r="B233" s="1"/>
       <c r="C233" s="10"/>
@@ -3880,9 +3637,8 @@
       <c r="I233" s="1"/>
       <c r="J233" s="1"/>
       <c r="K233" s="1"/>
-      <c r="L233" s="1"/>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="10"/>
       <c r="B234" s="1"/>
       <c r="C234" s="10"/>
@@ -3894,9 +3650,8 @@
       <c r="I234" s="1"/>
       <c r="J234" s="1"/>
       <c r="K234" s="1"/>
-      <c r="L234" s="1"/>
-    </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="10"/>
       <c r="B235" s="1"/>
       <c r="C235" s="10"/>
@@ -3908,9 +3663,8 @@
       <c r="I235" s="1"/>
       <c r="J235" s="1"/>
       <c r="K235" s="1"/>
-      <c r="L235" s="1"/>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="10"/>
       <c r="B236" s="1"/>
       <c r="C236" s="10"/>
@@ -3922,9 +3676,8 @@
       <c r="I236" s="1"/>
       <c r="J236" s="1"/>
       <c r="K236" s="1"/>
-      <c r="L236" s="1"/>
-    </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="10"/>
       <c r="B237" s="1"/>
       <c r="C237" s="10"/>
@@ -3936,9 +3689,8 @@
       <c r="I237" s="1"/>
       <c r="J237" s="1"/>
       <c r="K237" s="1"/>
-      <c r="L237" s="1"/>
-    </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="10"/>
       <c r="B238" s="1"/>
       <c r="C238" s="10"/>
@@ -3950,9 +3702,8 @@
       <c r="I238" s="1"/>
       <c r="J238" s="1"/>
       <c r="K238" s="1"/>
-      <c r="L238" s="1"/>
-    </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="10"/>
       <c r="B239" s="1"/>
       <c r="C239" s="10"/>
@@ -3964,9 +3715,8 @@
       <c r="I239" s="1"/>
       <c r="J239" s="1"/>
       <c r="K239" s="1"/>
-      <c r="L239" s="1"/>
-    </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="10"/>
       <c r="B240" s="1"/>
       <c r="C240" s="10"/>
@@ -3978,9 +3728,8 @@
       <c r="I240" s="1"/>
       <c r="J240" s="1"/>
       <c r="K240" s="1"/>
-      <c r="L240" s="1"/>
-    </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="10"/>
       <c r="B241" s="1"/>
       <c r="C241" s="10"/>
@@ -3992,9 +3741,8 @@
       <c r="I241" s="1"/>
       <c r="J241" s="1"/>
       <c r="K241" s="1"/>
-      <c r="L241" s="1"/>
-    </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="10"/>
       <c r="B242" s="1"/>
       <c r="C242" s="10"/>
@@ -4006,9 +3754,8 @@
       <c r="I242" s="1"/>
       <c r="J242" s="1"/>
       <c r="K242" s="1"/>
-      <c r="L242" s="1"/>
-    </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="10"/>
       <c r="B243" s="1"/>
       <c r="C243" s="10"/>
@@ -4020,9 +3767,8 @@
       <c r="I243" s="1"/>
       <c r="J243" s="1"/>
       <c r="K243" s="1"/>
-      <c r="L243" s="1"/>
-    </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="10"/>
       <c r="B244" s="1"/>
       <c r="C244" s="10"/>
@@ -4034,9 +3780,8 @@
       <c r="I244" s="1"/>
       <c r="J244" s="1"/>
       <c r="K244" s="1"/>
-      <c r="L244" s="1"/>
-    </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="10"/>
       <c r="B245" s="1"/>
       <c r="C245" s="10"/>
@@ -4048,9 +3793,8 @@
       <c r="I245" s="1"/>
       <c r="J245" s="1"/>
       <c r="K245" s="1"/>
-      <c r="L245" s="1"/>
-    </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="10"/>
       <c r="B246" s="1"/>
       <c r="C246" s="10"/>
@@ -4062,9 +3806,8 @@
       <c r="I246" s="1"/>
       <c r="J246" s="1"/>
       <c r="K246" s="1"/>
-      <c r="L246" s="1"/>
-    </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="10"/>
       <c r="B247" s="1"/>
       <c r="C247" s="10"/>
@@ -4076,9 +3819,8 @@
       <c r="I247" s="1"/>
       <c r="J247" s="1"/>
       <c r="K247" s="1"/>
-      <c r="L247" s="1"/>
-    </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="10"/>
       <c r="B248" s="1"/>
       <c r="C248" s="10"/>
@@ -4090,9 +3832,8 @@
       <c r="I248" s="1"/>
       <c r="J248" s="1"/>
       <c r="K248" s="1"/>
-      <c r="L248" s="1"/>
-    </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="10"/>
       <c r="B249" s="1"/>
       <c r="C249" s="10"/>
@@ -4104,9 +3845,8 @@
       <c r="I249" s="1"/>
       <c r="J249" s="1"/>
       <c r="K249" s="1"/>
-      <c r="L249" s="1"/>
-    </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="10"/>
       <c r="B250" s="1"/>
       <c r="C250" s="10"/>
@@ -4118,7 +3858,6 @@
       <c r="I250" s="1"/>
       <c r="J250" s="1"/>
       <c r="K250" s="1"/>
-      <c r="L250" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4130,7 +3869,7 @@
           <x14:formula1>
             <xm:f>'Mã ngành nghề '!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4154,66 +3893,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4221,7 +3960,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>